<commit_message>
Finished my portion of uts
utVendAddress
utVendor
utVendorAddr
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/VendAddress.xlsx
+++ b/UT.Vend.BLL/HelperFiles/VendAddress.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Table</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Toronto</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>2632 Marine Way</t>
@@ -239,13 +242,16 @@
       <c r="H2">
         <v>94043</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c t="str" r="M2">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('1','1600 Amphitheatre Pkwy','','','Mountain View','CA','94043','','0')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('1','1600 Amphitheatre Pkwy','','','Mountain View','CA','94043','0','0')</v>
       </c>
     </row>
     <row r="3">
@@ -267,13 +273,16 @@
       <c r="H3">
         <v>19108</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
       <c r="J3">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c t="str" r="M3">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('2','401 N Broad St','','','Philadelphia','PA','19108','','0')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('2','401 N Broad St','','','Philadelphia','PA','19108','0','0')</v>
       </c>
     </row>
     <row r="4">
@@ -295,13 +304,16 @@
       <c r="H4">
         <v>2108</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
       <c r="J4">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c t="str" r="M4">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('3','One Beacon Street','','','Boston','MA','2108','','0')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('3','One Beacon Street','','','Boston','MA','2108','0','0')</v>
       </c>
     </row>
     <row r="5">
@@ -323,13 +335,16 @@
       <c r="H5">
         <v>19119</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
       <c r="J5">
         <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="str" r="M5">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('4','7151 Germantown Ave','','','Philadelphia','PA','19119','','1')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('4','7151 Germantown Ave','','','Philadelphia','PA','19119','0','0')</v>
       </c>
     </row>
     <row r="6">
@@ -351,13 +366,16 @@
       <c r="H6">
         <v>60197</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
       <c r="J6">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c t="str" r="M6">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('5','PO Box 6577','','','Carol Stream','IL','60197','','0')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('5','PO Box 6577','','','Carol Stream','IL','60197','0','0')</v>
       </c>
     </row>
     <row r="7">
@@ -379,13 +397,16 @@
       <c r="H7">
         <v>94080</v>
       </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
       <c r="J7">
         <f>RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c t="str" r="M7">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('6','1 DNA Way','','','South San Francisco','CA','94080','','1')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('6','1 DNA Way','','','South San Francisco','CA','94080','0','1')</v>
       </c>
     </row>
     <row r="8">
@@ -401,16 +422,22 @@
       <c t="s" r="F8">
         <v>30</v>
       </c>
+      <c t="s" r="G8">
+        <v>31</v>
+      </c>
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
       <c r="J8">
         <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="str" r="M8">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('7','20 Bay St.','','','Toronto','','0','','1')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('7','20 Bay St.','','','Toronto','NA','0','0','0')</v>
       </c>
     </row>
     <row r="9">
@@ -421,7 +448,7 @@
         <v>8</v>
       </c>
       <c t="s" r="C9">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c t="s" r="F9">
         <v>15</v>
@@ -432,13 +459,16 @@
       <c r="H9">
         <v>94043</v>
       </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
       <c r="J9">
         <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="str" r="M9">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('8','2632 Marine Way','','','Mountain View','CA','94043','','1')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('8','2632 Marine Way','','','Mountain View','CA','94043','0','0')</v>
       </c>
     </row>
     <row r="10">
@@ -449,7 +479,7 @@
         <v>9</v>
       </c>
       <c t="s" r="C10">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c t="s" r="F10">
         <v>18</v>
@@ -460,13 +490,16 @@
       <c r="H10">
         <v>19103</v>
       </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
       <c r="J10">
         <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="str" r="M10">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('9','1818 Market St','','','Philadelphia','PA','19103','','1')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('9','1818 Market St','','','Philadelphia','PA','19103','0','0')</v>
       </c>
     </row>
     <row r="11">
@@ -477,10 +510,10 @@
         <v>10</v>
       </c>
       <c t="s" r="C11">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c t="s" r="F11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c t="s" r="G11">
         <v>16</v>
@@ -488,13 +521,16 @@
       <c r="H11">
         <v>94063</v>
       </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
       <c r="J11">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c t="str" r="M11">
         <f>((((((((((((((((((((((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ",") &amp; $G$1) &amp; ",") &amp; $H$1) &amp; ",") &amp; $I$1) &amp; ",") &amp; $J$1)  &amp; ") VALUES('") &amp; RC[-11]) &amp;"','") &amp; RC[-10]) &amp;"','") &amp; RC[-9]) &amp;"','") &amp; RC[-8]) &amp;"','") &amp; RC[-7]) &amp;"") &amp;"','") &amp; RC[-6]) &amp;"") &amp;"','") &amp; RC[-5]) &amp;"") &amp;"','") &amp; RC[-4]) &amp;"") &amp;"','") &amp; RC[-3]) &amp;"')"</f>
-        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('10','1450 Veterans Blvd','','','Redwood City','CA','94063','','0')</v>
+        <v>INSERT INTO [VolTeer].[Vend].[tblVendAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('10','1450 Veterans Blvd','','','Redwood City','CA','94063','0','0')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>